<commit_message>
Test files and test cases updated with valid codeValues
</commit_message>
<xml_diff>
--- a/test_files/Draft_Code_list_without_codes.xlsx
+++ b/test_files/Draft_Code_list_without_codes.xlsx
@@ -79,7 +79,7 @@
     <t>LICENSE</t>
   </si>
   <si>
-    <t>Koodisto 6000</t>
+    <t>Koodisto6000</t>
   </si>
   <si>
     <t>P1;P10;P11</t>
@@ -116,27 +116,15 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-    </font>
-    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -159,30 +147,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -202,11 +181,8 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="2" max="2" width="17.71"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="18.75">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -274,55 +250,55 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" ht="18.75">
-      <c r="A2" s="2" t="s">
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="1">
         <v>1.0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="3"/>
       <c r="M2" s="1" t="s">
         <v>29</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="6"/>
+      <c r="O2" s="3"/>
       <c r="P2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="4">
         <v>43161.0</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2" s="4">
         <v>43189.0</v>
       </c>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>